<commit_message>
Add documentation package for external review
- TECHNICAL_DOCS.md: Comprehensive maintenance manual with architecture,
  data flow, function reference, and troubleshooting guides
- R_PACKAGES.md: Package dependencies with justifications and security notes
- Enhanced CatDriver_Config_Template.xlsx: 4-sheet template with Settings,
  Variables, Instructions, and Effect Size Guide
</commit_message>
<xml_diff>
--- a/templates/CatDriver_Config_Template.xlsx
+++ b/templates/CatDriver_Config_Template.xlsx
@@ -9,6 +9,8 @@
   <sheets>
     <sheet name="Settings" sheetId="1" state="visible" r:id="rId1"/>
     <sheet name="Variables" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet name="Instructions" sheetId="3" state="visible" r:id="rId3"/>
+    <sheet name="Effect Size Guide" sheetId="4" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -18,7 +20,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="1">
+  <fonts count="5">
     <font>
       <name val="Calibri"/>
       <family val="2"/>
@@ -26,16 +28,62 @@
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <b val="1"/>
+      <color rgb="00FFFFFF"/>
+    </font>
+    <font>
+      <b val="1"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <color rgb="004472C4"/>
+      <sz val="14"/>
+    </font>
+    <font>
+      <b val="1"/>
+      <sz val="12"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="7">
     <fill>
       <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="004472C4"/>
+        <bgColor rgb="004472C4"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FFF2CC"/>
+        <bgColor rgb="00FFF2CC"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00E2EFDA"/>
+        <bgColor rgb="00E2EFDA"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00DDEBF7"/>
+        <bgColor rgb="00DDEBF7"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="00FCE4D6"/>
+        <bgColor rgb="00FCE4D6"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -43,12 +91,40 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" pivotButton="0" quotePrefix="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0" hidden="0"/>
@@ -414,177 +490,335 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:C10"/>
+  <dimension ref="A1:F10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="35" customWidth="1" min="2" max="2"/>
+    <col width="10" customWidth="1" min="3" max="3"/>
+    <col width="20" customWidth="1" min="4" max="4"/>
+    <col width="50" customWidth="1" min="5" max="5"/>
+    <col width="30" customWidth="1" min="6" max="6"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>Setting</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Value</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
+        <is>
+          <t>Required</t>
+        </is>
+      </c>
+      <c r="D1" s="1" t="inlineStr">
+        <is>
+          <t>Default</t>
+        </is>
+      </c>
+      <c r="E1" s="1" t="inlineStr">
         <is>
           <t>Description</t>
         </is>
       </c>
+      <c r="F1" s="1" t="inlineStr">
+        <is>
+          <t>Valid Values</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>analysis_name</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="2" t="inlineStr">
         <is>
           <t>My Categorical Key Driver Analysis</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>Name for this analysis (appears in output)</t>
+      <c r="C2" s="2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D2" s="2" t="inlineStr">
+        <is>
+          <t>Key Driver Analysis</t>
+        </is>
+      </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>Display name for this analysis (appears in reports)</t>
+        </is>
+      </c>
+      <c r="F2" s="2" t="inlineStr">
+        <is>
+          <t>Any text</t>
         </is>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>data_file</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="2" t="inlineStr">
         <is>
           <t>data.csv</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>Path to data file (relative to config or absolute)</t>
+      <c r="C3" s="3" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="D3" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>Path to data file. Can be relative (from config location) or absolute</t>
+        </is>
+      </c>
+      <c r="F3" s="2" t="inlineStr">
+        <is>
+          <t>.csv, .xlsx, .xls, .sav, .dta</t>
         </is>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="inlineStr">
+      <c r="A4" s="2" t="inlineStr">
         <is>
           <t>output_file</t>
         </is>
       </c>
-      <c r="B4" t="inlineStr">
+      <c r="B4" s="2" t="inlineStr">
         <is>
           <t>output/catdriver_results.xlsx</t>
         </is>
       </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Path for output Excel file</t>
+      <c r="C4" s="3" t="inlineStr">
+        <is>
+          <t>YES</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr">
+        <is>
+          <t>-</t>
+        </is>
+      </c>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>Path for output Excel file. Directory will be created if needed</t>
+        </is>
+      </c>
+      <c r="F4" s="2" t="inlineStr">
+        <is>
+          <t>.xlsx path</t>
         </is>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="inlineStr">
+      <c r="A5" s="2" t="inlineStr">
         <is>
           <t>outcome_type</t>
         </is>
       </c>
-      <c r="B5" t="inlineStr">
+      <c r="B5" s="2" t="inlineStr">
         <is>
           <t>auto</t>
         </is>
       </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>auto/binary/ordinal/nominal - override auto-detection</t>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr">
+        <is>
+          <t>auto</t>
+        </is>
+      </c>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>Override automatic outcome type detection</t>
+        </is>
+      </c>
+      <c r="F5" s="2" t="inlineStr">
+        <is>
+          <t>auto | binary | ordinal | nominal</t>
         </is>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
+      <c r="A6" s="2" t="inlineStr">
         <is>
           <t>reference_category</t>
         </is>
       </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Reference category for outcome (blank = auto)</t>
+      <c r="B6" s="2" t="inlineStr"/>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr">
+        <is>
+          <t>First alphabetically</t>
+        </is>
+      </c>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>Reference category for outcome comparisons (leave blank for auto)</t>
+        </is>
+      </c>
+      <c r="F6" s="2" t="inlineStr">
+        <is>
+          <t>Category name from outcome variable</t>
         </is>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="inlineStr">
+      <c r="A7" s="2" t="inlineStr">
         <is>
           <t>min_sample_size</t>
         </is>
       </c>
-      <c r="B7" t="inlineStr">
+      <c r="B7" s="2" t="inlineStr">
         <is>
           <t>30</t>
         </is>
       </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>Minimum complete cases required</t>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="inlineStr">
+        <is>
+          <t>30</t>
+        </is>
+      </c>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>Minimum complete cases required to run analysis</t>
+        </is>
+      </c>
+      <c r="F7" s="2" t="inlineStr">
+        <is>
+          <t>Positive integer (recommend 30+)</t>
         </is>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="inlineStr">
+      <c r="A8" s="2" t="inlineStr">
         <is>
           <t>confidence_level</t>
         </is>
       </c>
-      <c r="B8" t="inlineStr">
+      <c r="B8" s="2" t="inlineStr">
         <is>
           <t>0.95</t>
         </is>
       </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>Confidence level for intervals (0.95 = 95%)</t>
+      <c r="C8" s="2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D8" s="2" t="inlineStr">
+        <is>
+          <t>0.95</t>
+        </is>
+      </c>
+      <c r="E8" s="2" t="inlineStr">
+        <is>
+          <t>Confidence level for intervals (0.95 = 95% CI)</t>
+        </is>
+      </c>
+      <c r="F8" s="2" t="inlineStr">
+        <is>
+          <t>0.80 to 0.99</t>
         </is>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="inlineStr">
+      <c r="A9" s="2" t="inlineStr">
         <is>
           <t>missing_threshold</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B9" s="2" t="inlineStr">
         <is>
           <t>50</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>Warn if any variable exceeds this % missing</t>
+      <c r="C9" s="2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D9" s="2" t="inlineStr">
+        <is>
+          <t>50</t>
+        </is>
+      </c>
+      <c r="E9" s="2" t="inlineStr">
+        <is>
+          <t>Warn if any variable has missing data above this percentage</t>
+        </is>
+      </c>
+      <c r="F9" s="2" t="inlineStr">
+        <is>
+          <t>0 to 100</t>
         </is>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="inlineStr">
+      <c r="A10" s="2" t="inlineStr">
         <is>
           <t>detailed_output</t>
         </is>
       </c>
-      <c r="B10" t="inlineStr">
+      <c r="B10" s="2" t="inlineStr">
         <is>
           <t>TRUE</t>
         </is>
       </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>TRUE for 6 sheets, FALSE for 4 sheets</t>
+      <c r="C10" s="2" t="inlineStr">
+        <is>
+          <t>No</t>
+        </is>
+      </c>
+      <c r="D10" s="2" t="inlineStr">
+        <is>
+          <t>TRUE</t>
+        </is>
+      </c>
+      <c r="E10" s="2" t="inlineStr">
+        <is>
+          <t>TRUE = 6 sheets (includes Odds Ratios &amp; Diagnostics). FALSE = 4 sheets</t>
+        </is>
+      </c>
+      <c r="F10" s="2" t="inlineStr">
+        <is>
+          <t>TRUE | FALSE</t>
         </is>
       </c>
     </row>
@@ -599,133 +833,843 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:E7"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="20" customWidth="1" min="1" max="1"/>
+    <col width="10" customWidth="1" min="2" max="2"/>
+    <col width="25" customWidth="1" min="3" max="3"/>
+    <col width="25" customWidth="1" min="4" max="4"/>
+    <col width="45" customWidth="1" min="5" max="5"/>
+  </cols>
   <sheetData>
     <row r="1">
-      <c r="A1" t="inlineStr">
+      <c r="A1" s="1" t="inlineStr">
         <is>
           <t>VariableName</t>
         </is>
       </c>
-      <c r="B1" t="inlineStr">
+      <c r="B1" s="1" t="inlineStr">
         <is>
           <t>Type</t>
         </is>
       </c>
-      <c r="C1" t="inlineStr">
+      <c r="C1" s="1" t="inlineStr">
         <is>
           <t>Label</t>
         </is>
       </c>
-      <c r="D1" t="inlineStr">
+      <c r="D1" s="1" t="inlineStr">
         <is>
           <t>Order</t>
         </is>
       </c>
+      <c r="E1" s="1" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
     </row>
     <row r="2">
-      <c r="A2" t="inlineStr">
+      <c r="A2" s="2" t="inlineStr">
         <is>
           <t>satisfaction</t>
         </is>
       </c>
-      <c r="B2" t="inlineStr">
+      <c r="B2" s="4" t="inlineStr">
         <is>
           <t>Outcome</t>
         </is>
       </c>
-      <c r="C2" t="inlineStr">
+      <c r="C2" s="2" t="inlineStr">
         <is>
           <t>Employment Satisfaction</t>
         </is>
       </c>
-      <c r="D2" t="inlineStr">
+      <c r="D2" s="2" t="inlineStr">
         <is>
           <t>Low;Neutral;High</t>
         </is>
       </c>
+      <c r="E2" s="2" t="inlineStr">
+        <is>
+          <t>The outcome variable you want to explain (exactly 1 required)</t>
+        </is>
+      </c>
     </row>
     <row r="3">
-      <c r="A3" t="inlineStr">
+      <c r="A3" s="2" t="inlineStr">
         <is>
           <t>grade</t>
         </is>
       </c>
-      <c r="B3" t="inlineStr">
+      <c r="B3" s="5" t="inlineStr">
         <is>
           <t>Driver</t>
         </is>
       </c>
-      <c r="C3" t="inlineStr">
+      <c r="C3" s="2" t="inlineStr">
         <is>
           <t>Academic Grade</t>
         </is>
       </c>
-      <c r="D3" t="inlineStr">
+      <c r="D3" s="2" t="inlineStr">
         <is>
           <t>D;C;B;A</t>
+        </is>
+      </c>
+      <c r="E3" s="2" t="inlineStr">
+        <is>
+          <t>Predictor variable - specify Order for ordinal variables</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="inlineStr">
+        <is>
+          <t>campus</t>
+        </is>
+      </c>
+      <c r="B4" s="5" t="inlineStr">
+        <is>
+          <t>Driver</t>
+        </is>
+      </c>
+      <c r="C4" s="2" t="inlineStr">
+        <is>
+          <t>Campus Location</t>
+        </is>
+      </c>
+      <c r="D4" s="2" t="inlineStr"/>
+      <c r="E4" s="2" t="inlineStr">
+        <is>
+          <t>Predictor variable - leave Order blank for nominal variables</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="inlineStr">
+        <is>
+          <t>course_type</t>
+        </is>
+      </c>
+      <c r="B5" s="5" t="inlineStr">
+        <is>
+          <t>Driver</t>
+        </is>
+      </c>
+      <c r="C5" s="2" t="inlineStr">
+        <is>
+          <t>Course Type</t>
+        </is>
+      </c>
+      <c r="D5" s="2" t="inlineStr"/>
+      <c r="E5" s="2" t="inlineStr">
+        <is>
+          <t>Driver variable with categories</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="inlineStr">
+        <is>
+          <t>employment_field</t>
+        </is>
+      </c>
+      <c r="B6" s="5" t="inlineStr">
+        <is>
+          <t>Driver</t>
+        </is>
+      </c>
+      <c r="C6" s="2" t="inlineStr">
+        <is>
+          <t>Employment Field</t>
+        </is>
+      </c>
+      <c r="D6" s="2" t="inlineStr"/>
+      <c r="E6" s="2" t="inlineStr">
+        <is>
+          <t>Another predictor variable</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="inlineStr">
+        <is>
+          <t>survey_weight</t>
+        </is>
+      </c>
+      <c r="B7" s="6" t="inlineStr">
+        <is>
+          <t>Weight</t>
+        </is>
+      </c>
+      <c r="C7" s="2" t="inlineStr">
+        <is>
+          <t>Survey Weight</t>
+        </is>
+      </c>
+      <c r="D7" s="2" t="inlineStr"/>
+      <c r="E7" s="2" t="inlineStr">
+        <is>
+          <t>Optional weight variable (max 1) - leave blank if unweighted</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:A48"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="80" customWidth="1" min="1" max="1"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="7" t="inlineStr">
+        <is>
+          <t>CATEGORICAL KEY DRIVER ANALYSIS - CONFIGURATION GUIDE</t>
+        </is>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="inlineStr">
+        <is>
+          <t>OVERVIEW</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>campus</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t>Driver</t>
-        </is>
-      </c>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>Campus Location</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr"/>
+          <t>This configuration file controls the Categorical Key Driver Analysis module.</t>
+        </is>
+      </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>course_type</t>
-        </is>
-      </c>
-      <c r="B5" t="inlineStr">
-        <is>
-          <t>Driver</t>
-        </is>
-      </c>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>Course Type</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr"/>
+          <t>The module identifies which factors drive categorical outcomes using logistic regression.</t>
+        </is>
+      </c>
     </row>
     <row r="6">
-      <c r="A6" t="inlineStr">
-        <is>
-          <t>survey_weight</t>
-        </is>
-      </c>
-      <c r="B6" t="inlineStr">
-        <is>
-          <t>Weight</t>
-        </is>
-      </c>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>Survey Weight</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr"/>
+      <c r="A6" t="inlineStr"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="8" t="inlineStr">
+        <is>
+          <t>QUICK START</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>1. Edit the Settings sheet with your file paths</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>2. Edit the Variables sheet with your variable definitions</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>3. Save this file</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>4. Run the analysis via GUI or R script</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="8" t="inlineStr">
+        <is>
+          <t>SETTINGS SHEET</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>- data_file: Path to your data (CSV, Excel, SPSS, Stata)</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>- output_file: Where to save the results Excel file</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>- outcome_type: Usually leave as 'auto' for automatic detection</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>- Paths can be relative (from this config file) or absolute</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="8" t="inlineStr">
+        <is>
+          <t>VARIABLES SHEET</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" t="inlineStr">
+        <is>
+          <t>- VariableName: Exact column name in your data file (case-sensitive)</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" t="inlineStr">
+        <is>
+          <t>- Type: Must be Outcome, Driver, or Weight</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" t="inlineStr">
+        <is>
+          <t>- Label: Human-readable name for reports</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" t="inlineStr">
+        <is>
+          <t>- Order: For ordinal variables, list categories from lowest to highest</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" t="inlineStr">
+        <is>
+          <t xml:space="preserve">         Separate with semicolons: Low;Medium;High</t>
+        </is>
+      </c>
+    </row>
+    <row r="25">
+      <c r="A25" t="inlineStr">
+        <is>
+          <t xml:space="preserve">         Leave blank for nominal (unordered) variables</t>
+        </is>
+      </c>
+    </row>
+    <row r="26">
+      <c r="A26" t="inlineStr"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="8" t="inlineStr">
+        <is>
+          <t>VARIABLE TYPES</t>
+        </is>
+      </c>
+    </row>
+    <row r="28">
+      <c r="A28" t="inlineStr">
+        <is>
+          <t>Outcome - The dependent variable you want to explain (exactly 1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="29">
+      <c r="A29" t="inlineStr">
+        <is>
+          <t>Driver  - Predictor variables that may influence the outcome (1+)</t>
+        </is>
+      </c>
+    </row>
+    <row r="30">
+      <c r="A30" t="inlineStr">
+        <is>
+          <t>Weight  - Optional survey weight variable (0 or 1)</t>
+        </is>
+      </c>
+    </row>
+    <row r="31">
+      <c r="A31" t="inlineStr"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="8" t="inlineStr">
+        <is>
+          <t>OUTCOME TYPE DETECTION</t>
+        </is>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>auto    - Module detects based on data characteristics</t>
+        </is>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>binary  - Exactly 2 categories (Yes/No, Success/Failure)</t>
+        </is>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>ordinal - 3+ ordered categories (Low/Medium/High)</t>
+        </is>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>nominal - 3+ unordered categories (Brand A/B/C/D)</t>
+        </is>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="8" t="inlineStr">
+        <is>
+          <t>ORDER COLUMN EXAMPLES</t>
+        </is>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Satisfaction levels:  Low;Neutral;High</t>
+        </is>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>Likert scale:         Strongly Disagree;Disagree;Neutral;Agree;Strongly Agree</t>
+        </is>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Letter grades:        F;D;C;B;A</t>
+        </is>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Numeric codes:        1;2;3;4;5</t>
+        </is>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="8" t="inlineStr">
+        <is>
+          <t>TIPS</t>
+        </is>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>- Use relative paths so projects work when moved to OneDrive</t>
+        </is>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>- The first category in Order becomes the reference for ordinal</t>
+        </is>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>- For nominal variables, first alphabetically is the reference</t>
+        </is>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>- Check spelling of variable names exactly matches your data file</t>
+        </is>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:C24"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <cols>
+    <col width="35" customWidth="1" min="1" max="1"/>
+    <col width="35" customWidth="1" min="2" max="2"/>
+    <col width="35" customWidth="1" min="3" max="3"/>
+  </cols>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="7" t="inlineStr">
+        <is>
+          <t>INTERPRETING RESULTS</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" s="8" t="inlineStr">
+        <is>
+          <t>ODDS RATIO INTERPRETATION</t>
+        </is>
+      </c>
+    </row>
+    <row r="4">
+      <c r="A4" s="9" t="inlineStr">
+        <is>
+          <t>Odds Ratio Range</t>
+        </is>
+      </c>
+      <c r="B4" s="9" t="inlineStr">
+        <is>
+          <t>Effect Size</t>
+        </is>
+      </c>
+      <c r="C4" s="9" t="inlineStr">
+        <is>
+          <t>Interpretation</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="10" t="inlineStr">
+        <is>
+          <t>0.9 - 1.1</t>
+        </is>
+      </c>
+      <c r="B5" s="10" t="inlineStr">
+        <is>
+          <t>Negligible</t>
+        </is>
+      </c>
+      <c r="C5" s="10" t="inlineStr">
+        <is>
+          <t>No meaningful difference from reference</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="10" t="inlineStr">
+        <is>
+          <t>0.67 - 0.9 or 1.1 - 1.5</t>
+        </is>
+      </c>
+      <c r="B6" s="10" t="inlineStr">
+        <is>
+          <t>Small</t>
+        </is>
+      </c>
+      <c r="C6" s="10" t="inlineStr">
+        <is>
+          <t>Minor difference, may not be actionable</t>
+        </is>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="10" t="inlineStr">
+        <is>
+          <t>0.5 - 0.67 or 1.5 - 2.0</t>
+        </is>
+      </c>
+      <c r="B7" s="10" t="inlineStr">
+        <is>
+          <t>Medium</t>
+        </is>
+      </c>
+      <c r="C7" s="10" t="inlineStr">
+        <is>
+          <t>Meaningful difference worth attention</t>
+        </is>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="10" t="inlineStr">
+        <is>
+          <t>0.33 - 0.5 or 2.0 - 3.0</t>
+        </is>
+      </c>
+      <c r="B8" s="10" t="inlineStr">
+        <is>
+          <t>Large</t>
+        </is>
+      </c>
+      <c r="C8" s="10" t="inlineStr">
+        <is>
+          <t>Substantial difference, high priority</t>
+        </is>
+      </c>
+    </row>
+    <row r="9">
+      <c r="A9" s="10" t="inlineStr">
+        <is>
+          <t>&lt; 0.33 or &gt; 3.0</t>
+        </is>
+      </c>
+      <c r="B9" s="10" t="inlineStr">
+        <is>
+          <t>Very Large</t>
+        </is>
+      </c>
+      <c r="C9" s="10" t="inlineStr">
+        <is>
+          <t>Major difference, investigate thoroughly</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" s="8" t="inlineStr">
+        <is>
+          <t>IMPORTANCE PERCENTAGE INTERPRETATION</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="9" t="inlineStr">
+        <is>
+          <t>Importance %</t>
+        </is>
+      </c>
+      <c r="B12" s="9" t="inlineStr">
+        <is>
+          <t>Category</t>
+        </is>
+      </c>
+      <c r="C12" s="9" t="inlineStr">
+        <is>
+          <t>Meaning</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="10" t="inlineStr">
+        <is>
+          <t>&gt; 30%</t>
+        </is>
+      </c>
+      <c r="B13" s="10" t="inlineStr">
+        <is>
+          <t>Dominant driver</t>
+        </is>
+      </c>
+      <c r="C13" s="10" t="inlineStr">
+        <is>
+          <t>Primary focus area - this factor has the strongest influence</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="10" t="inlineStr">
+        <is>
+          <t>15 - 30%</t>
+        </is>
+      </c>
+      <c r="B14" s="10" t="inlineStr">
+        <is>
+          <t>Major driver</t>
+        </is>
+      </c>
+      <c r="C14" s="10" t="inlineStr">
+        <is>
+          <t>Significant influence - worth prioritizing</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="10" t="inlineStr">
+        <is>
+          <t>5 - 15%</t>
+        </is>
+      </c>
+      <c r="B15" s="10" t="inlineStr">
+        <is>
+          <t>Moderate driver</t>
+        </is>
+      </c>
+      <c r="C15" s="10" t="inlineStr">
+        <is>
+          <t>Notable but secondary influence</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="10" t="inlineStr">
+        <is>
+          <t>&lt; 5%</t>
+        </is>
+      </c>
+      <c r="B16" s="10" t="inlineStr">
+        <is>
+          <t>Minor driver</t>
+        </is>
+      </c>
+      <c r="C16" s="10" t="inlineStr">
+        <is>
+          <t>Limited impact - lower priority</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="8" t="inlineStr">
+        <is>
+          <t>MODEL FIT (McFadden R²)</t>
+        </is>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="9" t="inlineStr">
+        <is>
+          <t>R² Value</t>
+        </is>
+      </c>
+      <c r="B20" s="9" t="inlineStr">
+        <is>
+          <t>Interpretation</t>
+        </is>
+      </c>
+      <c r="C20" s="9" t="inlineStr">
+        <is>
+          <t>Notes</t>
+        </is>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="10" t="inlineStr">
+        <is>
+          <t>0.4+</t>
+        </is>
+      </c>
+      <c r="B21" s="10" t="inlineStr">
+        <is>
+          <t>Excellent fit</t>
+        </is>
+      </c>
+      <c r="C21" s="10" t="inlineStr">
+        <is>
+          <t>Model explains outcome very well</t>
+        </is>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="10" t="inlineStr">
+        <is>
+          <t>0.2 - 0.4</t>
+        </is>
+      </c>
+      <c r="B22" s="10" t="inlineStr">
+        <is>
+          <t>Good fit</t>
+        </is>
+      </c>
+      <c r="C22" s="10" t="inlineStr">
+        <is>
+          <t>Strong explanatory power for social science</t>
+        </is>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="10" t="inlineStr">
+        <is>
+          <t>0.1 - 0.2</t>
+        </is>
+      </c>
+      <c r="B23" s="10" t="inlineStr">
+        <is>
+          <t>Moderate fit</t>
+        </is>
+      </c>
+      <c r="C23" s="10" t="inlineStr">
+        <is>
+          <t>Useful but other factors likely at play</t>
+        </is>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="10" t="inlineStr">
+        <is>
+          <t>&lt; 0.1</t>
+        </is>
+      </c>
+      <c r="B24" s="10" t="inlineStr">
+        <is>
+          <t>Limited</t>
+        </is>
+      </c>
+      <c r="C24" s="10" t="inlineStr">
+        <is>
+          <t>Model has limited explanatory power</t>
+        </is>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>